<commit_message>
additional edits from EG
- fix the missing classes in Cook + Lake data
- remove the mv_exempt category from output
- minor edits to readmes
</commit_message>
<xml_diff>
--- a/resources/property classes.xlsx
+++ b/resources/property classes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/abahls_cmap_illinois_gov/Documents/Documents/github_repos/effective_property_tax/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2A60A013-1040-4DEC-B76C-0C647DD12EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF013571-E9D9-4AA3-8254-A6847BA48987}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{2A60A013-1040-4DEC-B76C-0C647DD12EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87BC2CD5-1BD5-4255-8696-96F6A218081D}"/>
   <bookViews>
     <workbookView xWindow="17445" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,8 @@
     <sheet name="will" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cook!$A$1:$G$150</definedName>
-    <definedName name="Export_Output_2" localSheetId="0">Cook!$A$1:$E$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cook!$A$1:$G$153</definedName>
+    <definedName name="Export_Output_2" localSheetId="0">Cook!$A$1:$E$137</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="345">
   <si>
     <t>overall_class</t>
   </si>
@@ -1071,13 +1071,22 @@
   </si>
   <si>
     <t>land_use_code</t>
+  </si>
+  <si>
+    <t>Commercial Incentive Land</t>
+  </si>
+  <si>
+    <t>5000-Locally Assessed Railroad</t>
+  </si>
+  <si>
+    <t>Greenhouse incentive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1108,6 +1117,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1145,10 +1162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1160,8 +1178,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1440,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3043,7 +3063,7 @@
         <v>527</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B130" si="1">TEXT(A67,"000")</f>
+        <f t="shared" ref="B67:B133" si="1">TEXT(A67,"000")</f>
         <v>527</v>
       </c>
       <c r="C67" t="s">
@@ -3568,23 +3588,23 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="1"/>
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C89" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D89" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E89" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F89">
-        <v>0.1</v>
+        <v>0.101743</v>
       </c>
       <c r="G89" t="s">
         <v>157</v>
@@ -3592,14 +3612,14 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="1"/>
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C90" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D90" t="s">
         <v>97</v>
@@ -3616,23 +3636,23 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="1"/>
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="C91" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D91" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E91" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F91">
-        <v>0.108333</v>
+        <v>0.1</v>
       </c>
       <c r="G91" t="s">
         <v>157</v>
@@ -3640,23 +3660,23 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="1"/>
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="C92" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D92" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E92" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F92">
-        <v>0.1</v>
+        <v>0.108333</v>
       </c>
       <c r="G92" t="s">
         <v>157</v>
@@ -3664,23 +3684,23 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="1"/>
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C93" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D93" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E93" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F93">
-        <v>0.108333</v>
+        <v>0.1</v>
       </c>
       <c r="G93" t="s">
         <v>157</v>
@@ -3688,14 +3708,14 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="1"/>
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D94" t="s">
         <v>102</v>
@@ -3712,14 +3732,14 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="1"/>
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C95" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D95" t="s">
         <v>102</v>
@@ -3736,14 +3756,14 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="1"/>
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="C96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D96" t="s">
         <v>102</v>
@@ -3760,14 +3780,14 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" si="1"/>
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D97" t="s">
         <v>102</v>
@@ -3784,23 +3804,23 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="1"/>
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C98" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D98" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E98" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F98">
-        <v>0.2</v>
+        <v>0.108333</v>
       </c>
       <c r="G98" t="s">
         <v>157</v>
@@ -3808,14 +3828,14 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="1"/>
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D99" t="s">
         <v>106</v>
@@ -3832,14 +3852,14 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="1"/>
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D100" t="s">
         <v>106</v>
@@ -3856,14 +3876,14 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="1"/>
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="C101" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D101" t="s">
         <v>106</v>
@@ -3880,38 +3900,38 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>717</v>
+        <v>693</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="1"/>
-        <v>717</v>
+        <v>693</v>
       </c>
       <c r="C102" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D102" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E102" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F102">
-        <v>0.101743</v>
+        <v>0.2</v>
       </c>
       <c r="G102" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="1"/>
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="C103" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D103" t="s">
         <v>109</v>
@@ -3928,14 +3948,14 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="1"/>
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D104" t="s">
         <v>109</v>
@@ -3952,14 +3972,14 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="1"/>
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="C105" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="D105" t="s">
         <v>109</v>
@@ -3976,14 +3996,14 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="1"/>
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C106" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D106" t="s">
         <v>109</v>
@@ -4000,14 +4020,14 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="1"/>
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C107" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D107" t="s">
         <v>109</v>
@@ -4024,14 +4044,14 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="1"/>
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C108" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D108" t="s">
         <v>109</v>
@@ -4048,20 +4068,20 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>746</v>
+        <v>731</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="1"/>
-        <v>746</v>
+        <v>731</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="D109" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E109" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F109">
         <v>0.101743</v>
@@ -4072,14 +4092,14 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="1"/>
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C110" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="D110" t="s">
         <v>114</v>
@@ -4096,14 +4116,14 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="1"/>
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="C111" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="D111" t="s">
         <v>114</v>
@@ -4120,14 +4140,14 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="1"/>
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="C112" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="D112" t="s">
         <v>114</v>
@@ -4144,14 +4164,14 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="1"/>
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="D113" t="s">
         <v>114</v>
@@ -4168,14 +4188,14 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="1"/>
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C114" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D114" t="s">
         <v>114</v>
@@ -4192,14 +4212,14 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="B115" t="str">
         <f t="shared" si="1"/>
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="C115" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D115" t="s">
         <v>114</v>
@@ -4216,20 +4236,20 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>790</v>
+        <v>774</v>
       </c>
       <c r="B116" t="str">
         <f t="shared" si="1"/>
-        <v>790</v>
+        <v>774</v>
       </c>
       <c r="C116" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D116" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E116" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F116">
         <v>0.101743</v>
@@ -4240,14 +4260,14 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B117" t="str">
         <f t="shared" si="1"/>
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C117" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D117" t="s">
         <v>109</v>
@@ -4264,14 +4284,14 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="1"/>
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C118" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="D118" t="s">
         <v>109</v>
@@ -4288,14 +4308,14 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="1"/>
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="C119" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D119" t="s">
         <v>109</v>
@@ -4312,14 +4332,14 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B120" t="str">
         <f t="shared" si="1"/>
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C120" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="D120" t="s">
         <v>109</v>
@@ -4336,20 +4356,20 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B121" t="str">
         <f t="shared" si="1"/>
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D121" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E121" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F121">
         <v>0.101743</v>
@@ -4360,17 +4380,17 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>817</v>
+        <v>800</v>
       </c>
       <c r="B122" t="str">
         <f t="shared" si="1"/>
-        <v>817</v>
+        <v>800</v>
       </c>
       <c r="C122" t="s">
-        <v>70</v>
-      </c>
-      <c r="D122" t="s">
-        <v>122</v>
+        <v>342</v>
+      </c>
+      <c r="D122">
+        <v>8</v>
       </c>
       <c r="E122" t="s">
         <v>123</v>
@@ -4384,14 +4404,14 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>823</v>
+        <v>801</v>
       </c>
       <c r="B123" t="str">
         <f t="shared" si="1"/>
-        <v>823</v>
+        <v>801</v>
       </c>
       <c r="C123" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D123" t="s">
         <v>122</v>
@@ -4408,14 +4428,14 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="B124" t="str">
         <f t="shared" si="1"/>
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="C124" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D124" t="s">
         <v>122</v>
@@ -4432,14 +4452,14 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="B125" t="str">
         <f t="shared" si="1"/>
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="C125" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="D125" t="s">
         <v>122</v>
@@ -4456,14 +4476,14 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B126" t="str">
         <f t="shared" si="1"/>
-        <v>829</v>
-      </c>
-      <c r="C126" t="s">
-        <v>76</v>
+        <v>826</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="D126" t="s">
         <v>122</v>
@@ -4480,14 +4500,14 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B127" t="str">
         <f t="shared" si="1"/>
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C127" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D127" t="s">
         <v>122</v>
@@ -4504,14 +4524,14 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="1"/>
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="C128" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D128" t="s">
         <v>122</v>
@@ -4528,14 +4548,14 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="1"/>
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="C129" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D129" t="s">
         <v>122</v>
@@ -4552,17 +4572,17 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>880</v>
+        <v>830</v>
       </c>
       <c r="B130" t="str">
         <f t="shared" si="1"/>
-        <v>880</v>
+        <v>830</v>
       </c>
       <c r="C130" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D130" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E130" t="s">
         <v>123</v>
@@ -4571,22 +4591,22 @@
         <v>0.101743</v>
       </c>
       <c r="G130" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>881</v>
+        <v>831</v>
       </c>
       <c r="B131" t="str">
-        <f t="shared" ref="B131:B150" si="2">TEXT(A131,"000")</f>
-        <v>881</v>
+        <f t="shared" si="1"/>
+        <v>831</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D131" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E131" t="s">
         <v>123</v>
@@ -4595,469 +4615,544 @@
         <v>0.101743</v>
       </c>
       <c r="G131" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
+        <v>833</v>
+      </c>
+      <c r="B132" t="str">
+        <f t="shared" si="1"/>
+        <v>833</v>
+      </c>
+      <c r="C132" t="s">
+        <v>80</v>
+      </c>
+      <c r="D132" t="s">
+        <v>122</v>
+      </c>
+      <c r="E132" t="s">
+        <v>123</v>
+      </c>
+      <c r="F132">
+        <v>0.101743</v>
+      </c>
+      <c r="G132" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>880</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="1"/>
+        <v>880</v>
+      </c>
+      <c r="C133" t="s">
+        <v>85</v>
+      </c>
+      <c r="D133" t="s">
+        <v>126</v>
+      </c>
+      <c r="E133" t="s">
+        <v>123</v>
+      </c>
+      <c r="F133">
+        <v>0.101743</v>
+      </c>
+      <c r="G133" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>881</v>
+      </c>
+      <c r="B134" t="str">
+        <f t="shared" ref="B134:B153" si="2">TEXT(A134,"000")</f>
+        <v>881</v>
+      </c>
+      <c r="C134" t="s">
+        <v>105</v>
+      </c>
+      <c r="D134" t="s">
+        <v>126</v>
+      </c>
+      <c r="E134" t="s">
+        <v>123</v>
+      </c>
+      <c r="F134">
+        <v>0.101743</v>
+      </c>
+      <c r="G134" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135">
         <v>883</v>
       </c>
-      <c r="B132" t="str">
+      <c r="B135" t="str">
         <f t="shared" si="2"/>
         <v>883</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C135" t="s">
         <v>80</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D135" t="s">
         <v>126</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E135" t="s">
         <v>123</v>
       </c>
-      <c r="F132">
+      <c r="F135">
         <v>0.101743</v>
       </c>
-      <c r="G132" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133">
+      <c r="G135" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136">
         <v>887</v>
       </c>
-      <c r="B133" t="str">
+      <c r="B136" t="str">
         <f t="shared" si="2"/>
         <v>887</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C136" t="s">
         <v>88</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D136" t="s">
         <v>126</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E136" t="s">
         <v>123</v>
       </c>
-      <c r="F133">
+      <c r="F136">
         <v>0.101743</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G136" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137">
         <v>889</v>
       </c>
-      <c r="B134" t="str">
+      <c r="B137" t="str">
         <f t="shared" si="2"/>
         <v>889</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C137" t="s">
         <v>89</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D137" t="s">
         <v>126</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E137" t="s">
         <v>123</v>
       </c>
-      <c r="F134">
+      <c r="F137">
         <v>0.101743</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G137" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138">
         <v>890</v>
       </c>
-      <c r="B135" t="str">
+      <c r="B138" t="str">
         <f t="shared" si="2"/>
         <v>890</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C138" t="s">
         <v>127</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D138" t="s">
         <v>126</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E138" t="s">
         <v>123</v>
       </c>
-      <c r="F135">
+      <c r="F138">
         <v>0.101743</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G138" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139">
         <v>891</v>
       </c>
-      <c r="B136" t="str">
+      <c r="B139" t="str">
         <f t="shared" si="2"/>
         <v>891</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C139" t="s">
         <v>117</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D139" t="s">
         <v>122</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E139" t="s">
         <v>123</v>
       </c>
-      <c r="F136">
+      <c r="F139">
         <v>0.101743</v>
       </c>
-      <c r="G136" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137">
+      <c r="G139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140">
         <v>892</v>
       </c>
-      <c r="B137" t="str">
+      <c r="B140" t="str">
         <f t="shared" si="2"/>
         <v>892</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C140" t="s">
         <v>92</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D140" t="s">
         <v>122</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E140" t="s">
         <v>123</v>
       </c>
-      <c r="F137">
+      <c r="F140">
         <v>0.101743</v>
       </c>
-      <c r="G137" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A138">
+      <c r="G140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141">
         <v>893</v>
       </c>
-      <c r="B138" t="str">
+      <c r="B141" t="str">
         <f t="shared" si="2"/>
         <v>893</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C141" t="s">
         <v>93</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D141" t="s">
         <v>126</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E141" t="s">
         <v>123</v>
       </c>
-      <c r="F138">
+      <c r="F141">
         <v>0.101743</v>
       </c>
-      <c r="G138" t="s">
+      <c r="G141" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A139">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142">
         <v>897</v>
       </c>
-      <c r="B139" t="str">
+      <c r="B142" t="str">
         <f t="shared" si="2"/>
         <v>897</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C142" t="s">
         <v>94</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D142" t="s">
         <v>122</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E142" t="s">
         <v>123</v>
       </c>
-      <c r="F139">
+      <c r="F142">
         <v>0.101743</v>
       </c>
-      <c r="G139" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A140">
+      <c r="G142" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143">
         <v>899</v>
       </c>
-      <c r="B140" t="str">
+      <c r="B143" t="str">
         <f t="shared" si="2"/>
         <v>899</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C143" t="s">
         <v>128</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D143" t="s">
         <v>126</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E143" t="s">
         <v>123</v>
       </c>
-      <c r="F140">
+      <c r="F143">
         <v>0.101743</v>
       </c>
-      <c r="G140" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A141">
+      <c r="G143" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144">
         <v>900</v>
       </c>
-      <c r="B141" t="str">
+      <c r="B144" t="str">
         <f t="shared" si="2"/>
         <v>900</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C144" t="s">
         <v>129</v>
       </c>
-      <c r="D141">
+      <c r="D144">
         <v>9</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E144" t="s">
         <v>130</v>
       </c>
-      <c r="F141">
+      <c r="F144">
         <v>0.1</v>
       </c>
-      <c r="G141" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A142">
+      <c r="G144" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145">
         <v>913</v>
       </c>
-      <c r="B142" t="str">
+      <c r="B145" t="str">
         <f t="shared" si="2"/>
         <v>913</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C145" t="s">
         <v>131</v>
       </c>
-      <c r="D142">
+      <c r="D145">
         <v>9</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E145" t="s">
         <v>130</v>
       </c>
-      <c r="F142">
+      <c r="F145">
         <v>0.1</v>
       </c>
-      <c r="G142" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A143">
+      <c r="G145" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146">
         <v>914</v>
       </c>
-      <c r="B143" t="str">
+      <c r="B146" t="str">
         <f t="shared" si="2"/>
         <v>914</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C146" t="s">
         <v>132</v>
       </c>
-      <c r="D143">
+      <c r="D146">
         <v>9</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E146" t="s">
         <v>130</v>
       </c>
-      <c r="F143">
+      <c r="F146">
         <v>0.1</v>
       </c>
-      <c r="G143" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A144">
+      <c r="G146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A147">
         <v>915</v>
       </c>
-      <c r="B144" t="str">
+      <c r="B147" t="str">
         <f t="shared" si="2"/>
         <v>915</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C147" t="s">
         <v>133</v>
       </c>
-      <c r="D144">
+      <c r="D147">
         <v>9</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E147" t="s">
         <v>130</v>
       </c>
-      <c r="F144">
+      <c r="F147">
         <v>0.1</v>
       </c>
-      <c r="G144" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A145">
+      <c r="G147" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148">
         <v>918</v>
       </c>
-      <c r="B145" t="str">
+      <c r="B148" t="str">
         <f t="shared" si="2"/>
         <v>918</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C148" t="s">
         <v>134</v>
       </c>
-      <c r="D145">
+      <c r="D148">
         <v>9</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E148" t="s">
         <v>130</v>
       </c>
-      <c r="F145">
+      <c r="F148">
         <v>0.1</v>
       </c>
-      <c r="G145" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A146">
+      <c r="G148" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149">
         <v>919</v>
       </c>
-      <c r="B146" t="str">
+      <c r="B149" t="str">
         <f t="shared" si="2"/>
         <v>919</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C149" t="s">
         <v>135</v>
       </c>
-      <c r="D146">
+      <c r="D149">
         <v>9</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E149" t="s">
         <v>130</v>
       </c>
-      <c r="F146">
+      <c r="F149">
         <v>0.1</v>
       </c>
-      <c r="G146" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A147">
+      <c r="G149" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150">
         <v>990</v>
       </c>
-      <c r="B147" t="str">
+      <c r="B150" t="str">
         <f t="shared" si="2"/>
         <v>990</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C150" t="s">
         <v>136</v>
       </c>
-      <c r="D147">
+      <c r="D150">
         <v>9</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E150" t="s">
         <v>130</v>
       </c>
-      <c r="F147">
+      <c r="F150">
         <v>0.1</v>
       </c>
-      <c r="G147" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148">
+      <c r="G150" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151">
         <v>991</v>
       </c>
-      <c r="B148" t="str">
+      <c r="B151" t="str">
         <f t="shared" si="2"/>
         <v>991</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C151" t="s">
         <v>137</v>
       </c>
-      <c r="D148">
+      <c r="D151">
         <v>9</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E151" t="s">
         <v>130</v>
       </c>
-      <c r="F148">
+      <c r="F151">
         <v>0.1</v>
       </c>
-      <c r="G148" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149">
+      <c r="G151" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152">
         <v>996</v>
       </c>
-      <c r="B149" t="str">
+      <c r="B152" t="str">
         <f t="shared" si="2"/>
         <v>996</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C152" t="s">
         <v>46</v>
       </c>
-      <c r="D149">
+      <c r="D152">
         <v>9</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E152" t="s">
         <v>130</v>
       </c>
-      <c r="F149">
+      <c r="F152">
         <v>0.1</v>
       </c>
-      <c r="G149" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A150">
+      <c r="G152" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153">
         <v>997</v>
       </c>
-      <c r="B150" t="str">
+      <c r="B153" t="str">
         <f t="shared" si="2"/>
         <v>997</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C153" t="s">
         <v>47</v>
       </c>
-      <c r="D150">
+      <c r="D153">
         <v>9</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E153" t="s">
         <v>130</v>
       </c>
-      <c r="F150">
+      <c r="F153">
         <v>0.1</v>
       </c>
-      <c r="G150" t="s">
+      <c r="G153" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G150" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G153" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="C126" r:id="rId1" xr:uid="{5F41B9EB-67B4-46BF-880A-CFCA67EC1FE6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6027,10 +6122,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6063,7 +6158,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A23" si="0">LEFT(B3,2)</f>
+        <f t="shared" ref="A3:A24" si="0">LEFT(B3,2)</f>
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -6182,15 +6277,15 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>151</v>
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C13" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -6199,31 +6294,31 @@
         <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B15" t="s">
-        <v>330</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C16" t="s">
         <v>151</v>
@@ -6232,10 +6327,10 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C17" t="s">
         <v>151</v>
@@ -6244,22 +6339,22 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C19" t="s">
         <v>157</v>
@@ -6268,10 +6363,10 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C20" t="s">
         <v>157</v>
@@ -6280,10 +6375,10 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C21" t="s">
         <v>157</v>
@@ -6292,24 +6387,36 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C22" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
         <v>MH</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>338</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>